<commit_message>
Update to csv function
</commit_message>
<xml_diff>
--- a/Documents/Work Plan.xlsx
+++ b/Documents/Work Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Navy's class\Datasets\KPMG_Virtual_Internship_Challenge\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD01740-650E-4CF1-8F64-DF2B67B20E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF40706-480C-483D-940C-9A5CDEC889AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E5536037-9EFD-483A-9ABC-DB0E63419F41}"/>
+    <workbookView xWindow="-28275" yWindow="0" windowWidth="26895" windowHeight="15480" xr2:uid="{E5536037-9EFD-483A-9ABC-DB0E63419F41}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>Demographic, Addresses, Transactions</t>
   </si>
@@ -57,18 +57,6 @@
     <t>Data Exploration</t>
   </si>
   <si>
-    <t>(replace/ remove missing data, noises, inconsistencies,  remove duplicates, filter outliers, etc.)</t>
-  </si>
-  <si>
-    <t>( Pivot,  normalization, discretization/ binning, aggregation)</t>
-  </si>
-  <si>
-    <t>( Dimension reduction - PCA, Feature Selection)</t>
-  </si>
-  <si>
-    <t>( Stats, Correlations, Distribution, Clutering, etc.)</t>
-  </si>
-  <si>
     <t>Phase 2:</t>
   </si>
   <si>
@@ -124,18 +112,12 @@
   </si>
   <si>
     <t>( 3 dashboards: Customers, Purchases, Time-series)</t>
-  </si>
-  <si>
-    <t>( Customers age, generation, order_profit, recency, frequency, loyalty, etc.)</t>
   </si>
   <si>
     <t>Need more
  features ?</t>
   </si>
   <si>
-    <t>(Comebine all datasets, drop irrelevant columns,  feature Scaling, get dummies)</t>
-  </si>
-  <si>
     <t>Module 1</t>
   </si>
   <si>
@@ -155,6 +137,54 @@
   </si>
   <si>
     <t>Results Interpretation</t>
+  </si>
+  <si>
+    <t>( Check data skewness, Stats, Correlations, Distribution, Clutering, etc.)</t>
+  </si>
+  <si>
+    <t>(replace/ remove missing data, remove outliers, noises, inconsistencies,  remove duplicates, filter outliers, etc.)</t>
+  </si>
+  <si>
+    <t>( Customers age, generation, order_profit, recency, frequency, loyalty, time-series features, etc.)</t>
+  </si>
+  <si>
+    <t>(Comebine all datasets, drop irrelevant columns,  Normalization (L1/L2)/ Scaling, get dummies)</t>
+  </si>
+  <si>
+    <t>( Pivot, discretization/ binning (fixed width / quantile-based, aggregation, log/ quantile transform to reduce sknewness, split columns, etc.)</t>
+  </si>
+  <si>
+    <t>( Dimension reduction - PCA, Feature Importances)</t>
+  </si>
+  <si>
+    <t>Binning:</t>
+  </si>
+  <si>
+    <t>https://pbpython.com/pandas-qcut-cut.html</t>
+  </si>
+  <si>
+    <t>Pivot table:</t>
+  </si>
+  <si>
+    <t>https://pandas.pydata.org/docs/user_guide/reshaping.html</t>
+  </si>
+  <si>
+    <t>Aggregation:</t>
+  </si>
+  <si>
+    <t>https://pandas.pydata.org/pandas-docs/stable/reference/api/pandas.DataFrame.aggregate.html</t>
+  </si>
+  <si>
+    <t>Transformation</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/feature-transformation-for-multiple-linear-regression-in-python-8648ddf070b8</t>
+  </si>
+  <si>
+    <t>Transform methods:</t>
+  </si>
+  <si>
+    <t>https://www.marsja.se/transform-skewed-data-using-square-root-log-box-cox-methods-in-python/</t>
   </si>
 </sst>
 </file>
@@ -379,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -500,6 +530,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1055,16 +1091,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>703168</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>143436</xdr:rowOff>
+      <xdr:rowOff>176566</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>667912</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>892396</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>102197</xdr:rowOff>
+      <xdr:rowOff>135327</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1090,8 +1126,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6284818" y="6372786"/>
-          <a:ext cx="4526391" cy="4483136"/>
+          <a:off x="0" y="6280849"/>
+          <a:ext cx="4536744" cy="4721261"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1713,7 +1749,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="2915478" y="2078934"/>
-          <a:ext cx="7595152" cy="803414"/>
+          <a:ext cx="7876760" cy="911088"/>
           <a:chOff x="2915478" y="1888434"/>
           <a:chExt cx="7595152" cy="803414"/>
         </a:xfrm>
@@ -2398,10 +2434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5AB578-D33F-42F5-8932-29E4AB5EF39F}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,7 +2450,7 @@
     <col min="6" max="6" width="3.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="22.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="3" style="1" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="2.7109375" style="1" customWidth="1"/>
@@ -2422,7 +2458,7 @@
     <col min="14" max="14" width="2.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="18.5703125" style="1" customWidth="1"/>
     <col min="16" max="16" width="4.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" style="1" customWidth="1"/>
     <col min="18" max="18" width="2.42578125" style="1" customWidth="1"/>
     <col min="19" max="19" width="16.5703125" style="1" customWidth="1"/>
     <col min="20" max="20" width="2.7109375" style="1" customWidth="1"/>
@@ -2547,35 +2583,35 @@
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="37" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="36" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="37" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J6" s="17"/>
       <c r="K6" s="36" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="36" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="N6" s="17"/>
       <c r="O6" s="36" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="P6" s="17"/>
       <c r="Q6" s="36" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="R6" s="17"/>
       <c r="S6" s="18" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="T6" s="32"/>
     </row>
@@ -2617,11 +2653,11 @@
       </c>
       <c r="R7" s="12"/>
       <c r="S7" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="T7" s="32"/>
     </row>
-    <row r="8" spans="1:20" s="13" customFormat="1" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="13" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" s="20"/>
       <c r="C8" s="12"/>
@@ -2629,31 +2665,31 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="L8" s="12"/>
       <c r="M8" s="12" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="N8" s="12"/>
       <c r="O8" s="12" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="P8" s="12"/>
       <c r="Q8" s="12" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="R8" s="3"/>
       <c r="S8" s="21" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="T8" s="34"/>
     </row>
@@ -2663,29 +2699,29 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="38" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="38" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="38" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="38" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="38" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="38" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="R9" s="5"/>
       <c r="S9" s="23"/>
@@ -2694,38 +2730,38 @@
     <row r="10" spans="1:20" ht="52.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32"/>
       <c r="B10" s="22" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="P10" s="5"/>
       <c r="Q10" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="R10" s="5"/>
       <c r="S10" s="23"/>
@@ -2739,19 +2775,19 @@
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L11" s="14"/>
       <c r="M11" s="14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
@@ -2767,11 +2803,11 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="39" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="40" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -2790,18 +2826,18 @@
     <row r="13" spans="1:20" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="32"/>
       <c r="B13" s="26" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -2825,7 +2861,7 @@
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
       <c r="G14" s="30" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H14" s="29"/>
       <c r="I14" s="29"/>
@@ -2893,7 +2929,7 @@
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="G17" s="35" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H17" s="32"/>
       <c r="I17" s="32"/>
@@ -2909,14 +2945,14 @@
       <c r="S17" s="32"/>
       <c r="T17" s="32"/>
     </row>
-    <row r="18" spans="1:20" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
       <c r="D18" s="33"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
+      <c r="G18" s="33"/>
       <c r="H18" s="32"/>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
@@ -2931,29 +2967,137 @@
       <c r="S18" s="32"/>
       <c r="T18" s="32"/>
     </row>
-    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="32"/>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="T19" s="32"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
       <c r="T20" s="32"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="T21" s="32"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" s="42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J23" s="42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J24" s="42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J25" s="42"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J26" s="42"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J27" s="42"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J28" s="42"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J29" s="42"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J30" s="42"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J31" s="42"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J32" s="42"/>
+    </row>
+    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J33" s="42"/>
+    </row>
+    <row r="34" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J34" s="42"/>
+    </row>
+    <row r="35" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J35" s="42"/>
+    </row>
+    <row r="36" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J36" s="42"/>
+    </row>
+    <row r="37" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J37" s="42"/>
+    </row>
+    <row r="38" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J38" s="42"/>
+    </row>
+    <row r="39" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J39" s="42"/>
+    </row>
+    <row r="40" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J40" s="42"/>
+    </row>
+    <row r="41" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J41" s="42"/>
+    </row>
+    <row r="42" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J42" s="42"/>
+    </row>
+    <row r="43" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J43" s="42"/>
+    </row>
+    <row r="44" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J44" s="42"/>
+    </row>
+    <row r="45" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J45" s="42"/>
+    </row>
+    <row r="46" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J46" s="41"/>
+    </row>
+    <row r="47" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J47" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>